<commit_message>
corregidos todos los fallos
</commit_message>
<xml_diff>
--- a/src/main/resources/datosACargar.xlsx
+++ b/src/main/resources/datosACargar.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13770" windowHeight="3030"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -58,10 +58,10 @@
     <t>Q3318001I</t>
   </si>
   <si>
-    <t>43.36;-5.85</t>
-  </si>
-  <si>
-    <t>43.24;-5.78</t>
+    <t>43.36&amp;-5.85</t>
+  </si>
+  <si>
+    <t>43.24&amp;-5.78</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +405,7 @@
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -422,7 +422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -470,7 +470,10 @@
       <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>